<commit_message>
Finally plugged leak on line 997. Fixed camera direction forward
was not releasing the camera buffer before writing into it.
</commit_message>
<xml_diff>
--- a/Lab7/Zyrianov_Dmitrii_Rubric.xlsx
+++ b/Lab7/Zyrianov_Dmitrii_Rubric.xlsx
@@ -496,9 +496,6 @@
     <t>Student Confidence(X)</t>
   </si>
   <si>
-    <t xml:space="preserve">Student Name: DmitriiR </t>
-  </si>
-  <si>
     <t>Student Git Address: https://github.com/DmitriiR/Graphics2Project.git</t>
   </si>
   <si>
@@ -512,6 +509,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Student Name: Dmitrii Zyrianov</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1054,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -1150,10 +1150,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="8">
         <f t="shared" ref="G4:G35" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -1523,10 +1523,10 @@
         <v>3</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="8">
         <f t="shared" si="0"/>
@@ -1677,10 +1677,10 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
@@ -2163,10 +2163,10 @@
         <v>3</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G46" s="8">
         <f t="shared" si="1"/>
@@ -2321,10 +2321,10 @@
         <v>3</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G54" s="8">
         <f t="shared" si="1"/>
@@ -2350,10 +2350,10 @@
         <v>3</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G55" s="8">
         <f t="shared" si="1"/>
@@ -2550,10 +2550,10 @@
         <v>2</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G65" s="8">
         <f t="shared" si="1"/>
@@ -2579,10 +2579,10 @@
         <v>3</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G66" s="8">
         <f t="shared" si="1"/>
@@ -2633,10 +2633,10 @@
         <v>5</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G68" s="8">
         <f t="shared" ref="G68:G85" si="2" xml:space="preserve"> IF(EXACT(F68,"X"),IF(EXACT(E68,"I"),$B68,IF(EXACT(E68,"II"),$C68,IF(EXACT(E68,"III"),$D68,0))),0)</f>
@@ -3021,7 +3021,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3086,12 +3086,12 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -3179,7 +3179,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>